<commit_message>
Script TMPro update functioning
</commit_message>
<xml_diff>
--- a/tietokanta/class_progression/excel/class_progression_Bard.xlsx
+++ b/tietokanta/class_progression/excel/class_progression_Bard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\tietokanta\class_progression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\tietokanta\class_progression\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6611B1B-C902-4444-B4A5-2FFD2DB52739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEC930E-80E1-45D4-B4FE-36A47732F64C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -37,11 +37,14 @@
   <connection id="1" xr16:uid="{4A7C6F03-D9DE-444B-8706-1C0580DA75EF}" name="progression_schema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Riku\Koulu\Ohjelmointyo\tietokanta\class_progression\progression_schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="2" xr16:uid="{D7F0F89C-37F6-41C9-9BB9-4C925D178854}" name="progression_schema1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\Riku\Koulu\Ohjelmointyo\tietokanta\schemas\progression_schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="46">
   <si>
     <t>Ancestry</t>
   </si>
@@ -176,6 +179,9 @@
   </si>
   <si>
     <t>Advancement10</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -239,25 +245,25 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema1">
+  <Schema ID="Schema2">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Progressions">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Progression" form="unqualified">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="progression" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Level" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement1" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement2" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement3" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement4" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement5" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement6" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement7" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement8" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement9" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Advancement10" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="level" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement1" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement2" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement3" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement4" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement5" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement6" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement7" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement8" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement9" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="advancement10" form="unqualified"/>
                 </xsd:sequence>
               </xsd:complexType>
             </xsd:element>
@@ -266,48 +272,48 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="1" Name="Progressions-määritys" RootElement="Progressions" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  <Map ID="2" Name="Progressions-määritys" RootElement="Progressions" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B4D0F4B-AF1C-40E3-9253-43600BBC5B2C}" name="Taulukko1" displayName="Taulukko1" ref="A1:K21" tableType="xml" totalsRowShown="0" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B4D0F4B-AF1C-40E3-9253-43600BBC5B2C}" name="Taulukko1" displayName="Taulukko1" ref="A1:K21" tableType="xml" totalsRowShown="0" connectionId="2">
   <autoFilter ref="A1:K21" xr:uid="{A37D1FA2-5055-4A44-8F49-2D79D145D2A3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0A6ACF4A-087A-4B09-9C86-FEF985F60388}" uniqueName="Level" name="Level">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Level" xmlDataType="integer"/>
+    <tableColumn id="1" xr3:uid="{0A6ACF4A-087A-4B09-9C86-FEF985F60388}" uniqueName="level" name="Level">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/level" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{4B1F9446-57E5-4CF0-AC70-152E6E526637}" uniqueName="Advancement1" name="Advancement1">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement1" xmlDataType="string"/>
+    <tableColumn id="2" xr3:uid="{4B1F9446-57E5-4CF0-AC70-152E6E526637}" uniqueName="advancement1" name="Advancement1">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement1" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E6E21ABF-D388-492D-890B-8090066D5E8D}" uniqueName="Advancement2" name="Advancement2">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement2" xmlDataType="string"/>
+    <tableColumn id="3" xr3:uid="{E6E21ABF-D388-492D-890B-8090066D5E8D}" uniqueName="advancement2" name="Advancement2">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement2" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE2AF9E3-7A22-4DEE-B171-96FD75B2F83F}" uniqueName="Advancement3" name="Advancement3">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement3" xmlDataType="string"/>
+    <tableColumn id="4" xr3:uid="{AE2AF9E3-7A22-4DEE-B171-96FD75B2F83F}" uniqueName="advancement3" name="Advancement3">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement3" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3C97466E-5412-4B2F-B22B-3977174212FD}" uniqueName="Advancement4" name="Advancement4">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement4" xmlDataType="string"/>
+    <tableColumn id="5" xr3:uid="{3C97466E-5412-4B2F-B22B-3977174212FD}" uniqueName="advancement4" name="Advancement4">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement4" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B4B85C53-8A94-4B81-A956-164D39A215E5}" uniqueName="Advancement5" name="Advancement5">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement5" xmlDataType="string"/>
+    <tableColumn id="6" xr3:uid="{B4B85C53-8A94-4B81-A956-164D39A215E5}" uniqueName="advancement5" name="Advancement5">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement5" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5F68BC66-DE83-40C4-8711-E6090BC85EC4}" uniqueName="Advancement6" name="Advancement6">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement6" xmlDataType="string"/>
+    <tableColumn id="7" xr3:uid="{5F68BC66-DE83-40C4-8711-E6090BC85EC4}" uniqueName="advancement6" name="Advancement6">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement6" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CE875174-1610-48B3-B2DB-2FDB7320BB40}" uniqueName="Advancement7" name="Advancement7">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement7" xmlDataType="string"/>
+    <tableColumn id="8" xr3:uid="{CE875174-1610-48B3-B2DB-2FDB7320BB40}" uniqueName="advancement7" name="Advancement7">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement7" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B9862CA1-E8FA-4918-9C6C-7B1FF6827495}" uniqueName="Advancement8" name="Advancement8">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement8" xmlDataType="string"/>
+    <tableColumn id="9" xr3:uid="{B9862CA1-E8FA-4918-9C6C-7B1FF6827495}" uniqueName="advancement8" name="Advancement8">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement8" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E6736A42-03E2-4547-8342-AFCB19D4D76D}" uniqueName="Advancement9" name="Advancement9">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement9" xmlDataType="string"/>
+    <tableColumn id="10" xr3:uid="{E6736A42-03E2-4547-8342-AFCB19D4D76D}" uniqueName="advancement9" name="Advancement9">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement9" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A21ED764-4665-47B2-BBF0-A577B35D42D5}" uniqueName="Advancement10" name="Advancement10">
-      <xmlColumnPr mapId="1" xpath="/Progressions/Progression/Advancement10" xmlDataType="string"/>
+    <tableColumn id="11" xr3:uid="{A21ED764-4665-47B2-BBF0-A577B35D42D5}" uniqueName="advancement10" name="Advancement10">
+      <xmlColumnPr mapId="2" xpath="/Progressions/progression/advancement10" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -579,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,9 +657,15 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -665,14 +677,30 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -693,11 +721,21 @@
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -709,14 +747,30 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -734,12 +788,24 @@
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -751,14 +817,30 @@
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -776,12 +858,24 @@
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -793,14 +887,30 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -821,11 +931,21 @@
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -840,13 +960,27 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -867,11 +1001,21 @@
       <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -883,14 +1027,30 @@
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -911,11 +1071,21 @@
       <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -927,14 +1097,30 @@
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -955,11 +1141,21 @@
       <c r="F16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -971,14 +1167,30 @@
       <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -996,12 +1208,24 @@
       <c r="E18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1013,14 +1237,30 @@
       <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1038,12 +1278,24 @@
       <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1058,13 +1310,27 @@
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>